<commit_message>
Mise à jour des graphiques
</commit_message>
<xml_diff>
--- a/Resultats/Performance.xlsx
+++ b/Resultats/Performance.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierre-luctheriault/PycharmProjects/Projet3/Resultats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295FE778-FACA-4E45-B0A5-96948E550D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D17076-92BE-E44B-940E-6F2F958DDBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{06B29052-E754-C94E-80E9-DBD9D1F93434}"/>
   </bookViews>
   <sheets>
     <sheet name="N_x" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,10 +88,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,26 +409,26 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -437,13 +437,13 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -454,17 +454,17 @@
       <c r="B3">
         <v>14.6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>2.6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>48.1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f>100-(C3+D3)</f>
         <v>49.3</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -473,14 +473,14 @@
       <c r="B4">
         <v>18.600000000000001</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3.8</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f>3.1+57.2</f>
         <v>60.300000000000004</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f t="shared" ref="E4:E12" si="0">100-(C4+D4)</f>
         <v>35.899999999999991</v>
       </c>
@@ -492,14 +492,14 @@
       <c r="B5">
         <v>25.4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f>2.9+65.4</f>
         <v>68.300000000000011</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>27.599999999999994</v>
       </c>
@@ -511,14 +511,14 @@
       <c r="B6">
         <v>33.5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>3.7</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f>2.6+73.2</f>
         <v>75.8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
@@ -530,13 +530,13 @@
       <c r="B7">
         <v>45.6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>3.6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>81.5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>14.900000000000006</v>
       </c>
@@ -548,14 +548,14 @@
       <c r="B8">
         <v>87.21</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f>87.3+1.8</f>
         <v>89.1</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>7.9000000000000057</v>
       </c>
@@ -567,14 +567,14 @@
       <c r="B9">
         <v>140.143</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>2.5</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f>90.8+1.5</f>
         <v>92.3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>5.2000000000000028</v>
       </c>
@@ -586,13 +586,13 @@
       <c r="B10">
         <v>229.9</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>2.1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>94.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>3.4000000000000057</v>
       </c>
@@ -604,13 +604,13 @@
       <c r="B11">
         <v>701.7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>96.7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>2.2000000000000028</v>
       </c>
@@ -620,17 +620,17 @@
         <v>200</v>
       </c>
       <c r="B12">
-        <v>1161</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="D12" s="2">
+        <v>1101</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D12" s="1">
         <v>98.2</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000028</v>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>